<commit_message>
Add sanction and tariff scenarios
</commit_message>
<xml_diff>
--- a/analysis/4_run_message/scenarios_new.xlsx
+++ b/analysis/4_run_message/scenarios_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\message_trade\analysis\4_run_message\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FD3F70-4DD8-40E4-BC2B-AAE206EBDED0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA134C52-08FB-4502-A130-4A696912EE90}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5953306A-3E49-4D6C-A95F-65BD8AD6FB69}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="73">
   <si>
     <t>MESSAGE-TRADE Scenario and Version</t>
   </si>
@@ -244,6 +244,12 @@
   </si>
   <si>
     <t>Add coal</t>
+  </si>
+  <si>
+    <t>baseline</t>
+  </si>
+  <si>
+    <t>Distance and baseline tariffs in variable cost</t>
   </si>
 </sst>
 </file>
@@ -682,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8478204-7BB5-4095-9E62-D455880F0DDA}">
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1864,6 +1870,26 @@
         <v>70</v>
       </c>
     </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>71</v>
+      </c>
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" t="s">
+        <v>35</v>
+      </c>
+      <c r="F59" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:XFD1"/>

</xml_diff>